<commit_message>
Sesión 1 -  Notas actualizadas
</commit_message>
<xml_diff>
--- a/sesion01/s102.xlsx
+++ b/sesion01/s102.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonnomada/Documents/Cursos 2025/BELATRIX-EXCEL/curso/sesion01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B080241-C2C6-104C-AC07-AA6B8560EC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109D2380-772E-354F-B71D-E2A1E3292C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="2" xr2:uid="{41C7BBC0-CC87-4B41-A038-122ED8BC9960}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="3" xr2:uid="{41C7BBC0-CC87-4B41-A038-122ED8BC9960}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="19">
   <si>
     <t>Producto</t>
   </si>
@@ -169,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -257,16 +258,9 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <top style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -319,12 +313,6 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -334,12 +322,67 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1049,7 +1092,7 @@
   <dimension ref="B5:L23"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="136" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B5" sqref="B5:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1399,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F845CF1D-A56C-B940-B481-E68AF7781260}">
   <dimension ref="C4:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1611,7 +1654,7 @@
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="10" t="str" cm="1">
@@ -1642,7 +1685,7 @@
       </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="F16" s="18">
+      <c r="F16" s="16">
         <f>INDEX(C$5:D$10,MATCH(G16,C$5:C$10,0),2)</f>
         <v>39</v>
       </c>
@@ -1674,12 +1717,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="14">
-        <f>SUM(F16:M16)</f>
-        <v>429</v>
+        <f>SUM(H16:M16)</f>
+        <v>390</v>
       </c>
     </row>
     <row r="17" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="F17" s="18">
+      <c r="F17" s="16">
         <f>INDEX(C$5:D$10,MATCH(G17,C$5:C$10,0),2)</f>
         <v>48</v>
       </c>
@@ -1710,13 +1753,13 @@
         <f>INDEX($H$6:$M$11,MATCH(M$15,$G$6:$G$11, 0),MATCH($G17,$H$5:$M$5, 0))*$F17</f>
         <v>0</v>
       </c>
-      <c r="N17" s="15">
-        <f>SUM(F17:M17)</f>
-        <v>192</v>
+      <c r="N17" s="14">
+        <f t="shared" ref="N17:N21" si="0">SUM(H17:M17)</f>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="F18" s="18">
+      <c r="F18" s="16">
         <f>INDEX(C$5:D$10,MATCH(G18,C$5:C$10,0),2)</f>
         <v>21</v>
       </c>
@@ -1747,13 +1790,13 @@
         <f>INDEX($H$6:$M$11,MATCH(M$15,$G$6:$G$11, 0),MATCH($G18,$H$5:$M$5, 0))*$F18</f>
         <v>126</v>
       </c>
-      <c r="N18" s="15">
-        <f>SUM(F18:M18)</f>
-        <v>189</v>
+      <c r="N18" s="14">
+        <f t="shared" si="0"/>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="F19" s="18">
+      <c r="F19" s="16">
         <f>INDEX(C$5:D$10,MATCH(G19,C$5:C$10,0),2)</f>
         <v>34</v>
       </c>
@@ -1784,13 +1827,13 @@
         <f>INDEX($H$6:$M$11,MATCH(M$15,$G$6:$G$11, 0),MATCH($G19,$H$5:$M$5, 0))*$F19</f>
         <v>0</v>
       </c>
-      <c r="N19" s="15">
-        <f>SUM(F19:M19)</f>
-        <v>204</v>
+      <c r="N19" s="14">
+        <f t="shared" si="0"/>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="F20" s="18">
+      <c r="F20" s="16">
         <f>INDEX(C$5:D$10,MATCH(G20,C$5:C$10,0),2)</f>
         <v>85</v>
       </c>
@@ -1821,13 +1864,13 @@
         <f>INDEX($H$6:$M$11,MATCH(M$15,$G$6:$G$11, 0),MATCH($G20,$H$5:$M$5, 0))*$F20</f>
         <v>170</v>
       </c>
-      <c r="N20" s="15">
-        <f>SUM(F20:M20)</f>
-        <v>340</v>
+      <c r="N20" s="14">
+        <f t="shared" si="0"/>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="6:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="18">
+      <c r="F21" s="16">
         <f>INDEX(C$5:D$10,MATCH(G21,C$5:C$10,0),2)</f>
         <v>48</v>
       </c>
@@ -1858,43 +1901,714 @@
         <f>INDEX($H$6:$M$11,MATCH(M$15,$G$6:$G$11, 0),MATCH($G21,$H$5:$M$5, 0))*$F21</f>
         <v>0</v>
       </c>
-      <c r="N21" s="16">
-        <f>SUM(F21:M21)</f>
-        <v>240</v>
+      <c r="N21" s="19">
+        <f t="shared" si="0"/>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="F22" s="19"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="13" t="s">
         <v>17</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" ref="H22:N22" si="0">SUM(H16:H21)</f>
+        <f t="shared" ref="H22:N22" si="1">SUM(H16:H21)</f>
         <v>229</v>
       </c>
       <c r="I22" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>151</v>
       </c>
       <c r="J22" s="5">
+        <f t="shared" si="1"/>
+        <v>368</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" si="1"/>
+        <v>202</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" si="1"/>
+        <v>296</v>
+      </c>
+      <c r="N22" s="5">
+        <f t="shared" si="1"/>
+        <v>1319</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="N16:N21">
+    <cfRule type="aboveAverage" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:M22">
+    <cfRule type="aboveAverage" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703F3FAD-9FEB-4243-A4DB-60D80F0C0A0C}">
+  <dimension ref="A4:S24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" cm="1">
+        <f t="array" ref="M6:R6">TRANSPOSE(B$5:B$10)</f>
+        <v>39</v>
+      </c>
+      <c r="N6" s="2">
+        <v>48</v>
+      </c>
+      <c r="O6" s="2">
+        <v>21</v>
+      </c>
+      <c r="P6" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>85</v>
+      </c>
+      <c r="R6" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" cm="1">
+        <f t="array" ref="M7:R7">TRANSPOSE(B$5:B$10)</f>
+        <v>39</v>
+      </c>
+      <c r="N7" s="2">
+        <v>48</v>
+      </c>
+      <c r="O7" s="2">
+        <v>21</v>
+      </c>
+      <c r="P7" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>85</v>
+      </c>
+      <c r="R7" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="M8" s="2" cm="1">
+        <f t="array" ref="M8:R8">TRANSPOSE(B$5:B$10)</f>
+        <v>39</v>
+      </c>
+      <c r="N8" s="2">
+        <v>48</v>
+      </c>
+      <c r="O8" s="2">
+        <v>21</v>
+      </c>
+      <c r="P8" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>85</v>
+      </c>
+      <c r="R8" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" cm="1">
+        <f t="array" ref="M9:R9">TRANSPOSE(B$5:B$10)</f>
+        <v>39</v>
+      </c>
+      <c r="N9" s="2">
+        <v>48</v>
+      </c>
+      <c r="O9" s="2">
+        <v>21</v>
+      </c>
+      <c r="P9" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>85</v>
+      </c>
+      <c r="R9" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2" cm="1">
+        <f t="array" ref="M10:R10">TRANSPOSE(B$5:B$10)</f>
+        <v>39</v>
+      </c>
+      <c r="N10" s="2">
+        <v>48</v>
+      </c>
+      <c r="O10" s="2">
+        <v>21</v>
+      </c>
+      <c r="P10" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>85</v>
+      </c>
+      <c r="R10" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" cm="1">
+        <f t="array" ref="M11:R11">TRANSPOSE(B$5:B$10)</f>
+        <v>39</v>
+      </c>
+      <c r="N11" s="2">
+        <v>48</v>
+      </c>
+      <c r="O11" s="2">
+        <v>21</v>
+      </c>
+      <c r="P11" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>85</v>
+      </c>
+      <c r="R11" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="5:19" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" t="s">
+        <v>3</v>
+      </c>
+      <c r="P17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>5</v>
+      </c>
+      <c r="R17" t="s">
+        <v>6</v>
+      </c>
+      <c r="S17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="5:19" x14ac:dyDescent="0.2">
+      <c r="E18" cm="1">
+        <f t="array" ref="E18:J23">2*E6:J11</f>
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="L18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="2" cm="1">
+        <f t="array" ref="M18:R23">E6:J11*M6:R11</f>
+        <v>78</v>
+      </c>
+      <c r="N18" s="2">
+        <v>48</v>
+      </c>
+      <c r="O18" s="2">
+        <v>21</v>
+      </c>
+      <c r="P18" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>48</v>
+      </c>
+      <c r="S18" s="18">
+        <f>SUM(M18:R18)</f>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="5:19" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="2">
+        <v>117</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0</v>
+      </c>
+      <c r="S19" s="18">
+        <f t="shared" ref="S19:S24" si="0">SUM(M19:R19)</f>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="5:19" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="L20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="2">
+        <v>156</v>
+      </c>
+      <c r="N20" s="2">
+        <v>48</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2">
+        <v>68</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2">
+        <v>96</v>
+      </c>
+      <c r="S20" s="18">
         <f t="shared" si="0"/>
         <v>368</v>
       </c>
-      <c r="K22" s="5">
+    </row>
+    <row r="21" spans="5:19" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="2">
+        <v>39</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>0</v>
+      </c>
+      <c r="R21" s="2">
+        <v>0</v>
+      </c>
+      <c r="S21" s="18">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="L22" s="5">
+    </row>
+    <row r="22" spans="5:19" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="L22" t="s">
+        <v>12</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2">
+        <v>48</v>
+      </c>
+      <c r="O22" s="2">
+        <v>21</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>85</v>
+      </c>
+      <c r="R22" s="2">
+        <v>48</v>
+      </c>
+      <c r="S22" s="18">
         <f t="shared" si="0"/>
         <v>202</v>
       </c>
-      <c r="M22" s="5">
+    </row>
+    <row r="23" spans="5:19" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
+        <v>126</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>170</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0</v>
+      </c>
+      <c r="S23" s="18">
         <f t="shared" si="0"/>
         <v>296</v>
       </c>
-      <c r="N22" s="5">
+    </row>
+    <row r="24" spans="5:19" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="18">
+        <f>SUM(M18:M23)</f>
+        <v>390</v>
+      </c>
+      <c r="N24" s="18">
+        <f t="shared" ref="N24:S24" si="1">SUM(N18:N23)</f>
+        <v>144</v>
+      </c>
+      <c r="O24" s="18">
+        <f t="shared" si="1"/>
+        <v>168</v>
+      </c>
+      <c r="P24" s="18">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
+      <c r="Q24" s="18">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="R24" s="18">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="S24" s="18">
         <f t="shared" si="0"/>
-        <v>1594</v>
+        <v>1319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>